<commit_message>
update 10th of millis
</commit_message>
<xml_diff>
--- a/msgprotocol.xlsx
+++ b/msgprotocol.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="90" windowWidth="20730" windowHeight="11760"/>
+    <workbookView xWindow="0" yWindow="90" windowWidth="20730" windowHeight="11760" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Пример посылки" sheetId="1" r:id="rId1"/>
@@ -74,10 +74,10 @@
     <t xml:space="preserve"> - включить (любое число от 1 до 255) или выключить (0)</t>
   </si>
   <si>
-    <t xml:space="preserve"> - значение интервала времени (разрешены значения от 0 до 32767)</t>
+    <t xml:space="preserve"> - начало посылки интервала времени между отсчётами в десятых долях миллисекунды (не изменять)</t>
   </si>
   <si>
-    <t xml:space="preserve"> - начало посылки интервала времени между отсчётами в миллисекундах (не изменять)</t>
+    <t xml:space="preserve"> - значение интервала времени (разрешены значения от 1 до 160)</t>
   </si>
 </sst>
 </file>
@@ -546,7 +546,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A1010"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
@@ -5947,8 +5947,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H1011"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5966,7 +5966,7 @@
         <v>7</v>
       </c>
       <c r="C1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -5974,7 +5974,7 @@
         <v>555</v>
       </c>
       <c r="C2" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">

</xml_diff>